<commit_message>
2023/03/27 김진우 api 설계
</commit_message>
<xml_diff>
--- a/Photostagram API 설계.xlsx
+++ b/Photostagram API 설계.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java2\Desktop\Workspace\Photostagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimwoo2328/Desktop/Workspace/photostagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2785DAC-2934-6B46-A59F-703C4E68A12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18165" windowHeight="12015"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19460" windowHeight="13480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>구분</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,9 +110,6 @@
     <t>/Photostagram/index.do</t>
   </si>
   <si>
-    <t>/Photostagram/member/…</t>
-  </si>
-  <si>
     <t>/Photostagram/product/…</t>
   </si>
   <si>
@@ -131,12 +118,94 @@
   <si>
     <t>/Photostagram/admin/…</t>
   </si>
+  <si>
+    <t>/Photostagram/member/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/terms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/checkId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/checkPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/resultId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Photostagram/member/resultPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김진우</t>
+  </si>
+  <si>
+    <t>김진우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 가입 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 생일 입력 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 가입 이메일 인증 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 가입 이용약관 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 찾기 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 찾기 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 찾기 결과 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 찾기 임시 비밀번호 발송 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,18 +244,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
@@ -508,22 +571,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
-    <col min="2" max="2" width="33.375" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="43.125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +603,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -557,8 +620,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -572,71 +635,183 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -650,6 +825,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097CC9FFAC65EFA45BEA04EBBB60CAD5B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b23439a91ba18143205c49e90ab13d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60114a07b5dc583519299b7a26e1c8b6">
     <xsd:element name="properties">
@@ -763,12 +944,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -779,6 +954,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBE3480B-5504-4F1A-8E81-8AF0C8D9879C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E38BF8-DA76-4FEC-BE1F-43A93506C983}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -794,21 +984,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBE3480B-5504-4F1A-8E81-8AF0C8D9879C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{305CDDD2-5EEF-4FF9-9584-902F68B12982}">
   <ds:schemaRefs>

</xml_diff>